<commit_message>
update import Template RuleLinkFee
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Setting/eFMS.API.Setting/Resources/Files/RuleLinkFeeImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Setting/eFMS.API.Setting/Resources/Files/RuleLinkFeeImportTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Rule Name (*)</t>
   </si>
@@ -50,25 +50,22 @@
     <t>Status (*)</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>Sea Consol Export</t>
-  </si>
-  <si>
-    <t>EBS in VN</t>
-  </si>
-  <si>
-    <t>HANSOL VINA</t>
-  </si>
-  <si>
-    <t>VIET HY CO LTD</t>
-  </si>
-  <si>
     <t>Active</t>
   </si>
   <si>
-    <t>Phí di lý - Transfer fee</t>
+    <t>Rule import</t>
+  </si>
+  <si>
+    <t>Custom Logistic</t>
+  </si>
+  <si>
+    <t>BA_CHD_Air</t>
+  </si>
+  <si>
+    <t>SO_THC_OPS</t>
+  </si>
+  <si>
+    <t>USAOMNIUSA</t>
   </si>
 </sst>
 </file>
@@ -132,10 +129,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -460,29 +460,29 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3">
+        <v>162789394</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix col auto remove leading zeros on type numerics
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Setting/eFMS.API.Setting/Resources/Files/RuleLinkFeeImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Setting/eFMS.API.Setting/Resources/Files/RuleLinkFeeImportTemplate.xlsx
@@ -129,13 +129,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,40 +422,40 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="25" style="6" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -460,25 +463,25 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="5">
         <v>162789394</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">

</xml_diff>

<commit_message>
update import catch err
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Setting/eFMS.API.Setting/Resources/Files/RuleLinkFeeImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Setting/eFMS.API.Setting/Resources/Files/RuleLinkFeeImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.Setting\eFMS.API.Setting\Resources\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dane.dung\Documents\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.Setting\eFMS.API.Setting\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -56,9 +56,6 @@
     <t>Rule import</t>
   </si>
   <si>
-    <t>Custom Logistic</t>
-  </si>
-  <si>
     <t>BA_CHD_Air</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>USAOMNIUSA</t>
+  </si>
+  <si>
+    <t>CL</t>
   </si>
 </sst>
 </file>
@@ -129,10 +129,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -422,40 +420,41 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25" style="6" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25" style="4" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -463,26 +462,26 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="3">
+        <v>162789394</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="5">
-        <v>162789394</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>8</v>
@@ -490,5 +489,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>